<commit_message>
pushing for final time
</commit_message>
<xml_diff>
--- a/MavenVTigerProject/src/test/resources/VtigerData.xlsx
+++ b/MavenVTigerProject/src/test/resources/VtigerData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="153222"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15600" windowHeight="6195"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15600" windowHeight="6195" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="CampaiginData" sheetId="1" r:id="rId1"/>
@@ -12,7 +12,7 @@
     <sheet name="CreateLead" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A1:H18"/>
+  <oleSize ref="A1:L18"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -416,7 +416,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
@@ -471,7 +471,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C2" sqref="C2:C3"/>
     </sheetView>
   </sheetViews>

</xml_diff>